<commit_message>
[IMP] extras: Improve exported data documents.
</commit_message>
<xml_diff>
--- a/extras/data_extra/movies_jap_list_xlsx.xlsx
+++ b/extras/data_extra/movies_jap_list_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\repos\movies_lib_explorer-0\extras\data_extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22020B1-6971-49B8-B797-1B6CEF858255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222FC525-8048-4594-B084-F6EC1437EC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14922,9 +14922,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1375"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S4" sqref="S4"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>